<commit_message>
UPDATE 09.29.22 Clustering Model Completion
</commit_message>
<xml_diff>
--- a/Resources/Super Bowl Analysis.xlsx
+++ b/Resources/Super Bowl Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orich\Desktop\UM Fintech\1_UM_Repositories\Project_2_SuperBowlPrediction\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAD4584-4472-4863-B7CD-06A051AD3114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D77551-75E3-4208-8AF4-E3D451A0C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_2011_regular_ season_1" sheetId="1" r:id="rId1"/>
@@ -9757,7 +9757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D353"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -16493,7 +16493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UPDATE 09.30.22 - SuperBowl Analysis and Prediction
</commit_message>
<xml_diff>
--- a/Resources/Super Bowl Analysis.xlsx
+++ b/Resources/Super Bowl Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orich\Desktop\UM Fintech\1_UM_Repositories\Project_2_SuperBowlPrediction\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D77551-75E3-4208-8AF4-E3D451A0C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C088A6-F1A9-4DD6-B653-8085E39AA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_2011_regular_ season_1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="W" sheetId="3" r:id="rId3"/>
     <sheet name="Selection-W+Net Pts" sheetId="4" r:id="rId4"/>
     <sheet name="Consolidated" sheetId="5" r:id="rId5"/>
-    <sheet name="Sorted-Qualitative Knowledge" sheetId="6" r:id="rId6"/>
-    <sheet name="Final Listing" sheetId="7" r:id="rId7"/>
+    <sheet name="W3_Sorted-Qualitative Knowl (2)" sheetId="8" r:id="rId6"/>
+    <sheet name="W4_Sorted-Qualitative Knowledge" sheetId="6" r:id="rId7"/>
+    <sheet name="Final Listing" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2021_2011_regular_ season_1'!$A$1:$D$353</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="59">
   <si>
     <t>Years</t>
   </si>
@@ -223,12 +224,15 @@
   <si>
     <t>Super Bowl Championships</t>
   </si>
+  <si>
+    <t>https://www.pro-football-reference.com/years/2022/index.htm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +378,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -694,7 +706,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -737,8 +749,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -796,11 +809,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -834,6 +848,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -4711,10 +4726,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB1B8F0F-0132-393E-CBC1-8DC8EB0F2377}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90722C91-842E-474C-9F5E-8F719DA807A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4731,7 +4746,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4905375" y="190500"/>
-          <a:ext cx="12670018" cy="5506218"/>
+          <a:ext cx="12666843" cy="5506218"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9757,7 +9772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D353"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -16490,11 +16505,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062E0B44-D608-4A13-BD93-88B8CF0E4AC9}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -16703,13 +16718,13 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="20">
         <v>127</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="21">
         <v>90</v>
       </c>
       <c r="E13" s="3"/>
@@ -16761,7 +16776,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A17" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -16776,7 +16791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A18" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -16792,7 +16807,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A19" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -16808,7 +16823,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A20" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -16821,7 +16836,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A21" s="18">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -16834,7 +16849,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -16850,7 +16865,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A23" s="18">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -16863,7 +16878,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -16875,7 +16890,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A25" s="8">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -16893,7 +16908,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A26" s="8">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -16911,21 +16926,26 @@
         <v>54</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G29" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E26">
-    <sortCondition descending="1" ref="D2:D26"/>
-  </sortState>
+  <hyperlinks>
+    <hyperlink ref="G29" r:id="rId1" xr:uid="{1FFCCF5F-95BE-4C33-B224-E2ABC90A2DF9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -16944,20 +16964,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>1599</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="1">
         <v>128</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -16966,6 +16986,444 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1">
+        <v>708</v>
+      </c>
+      <c r="D3" s="17">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" s="8">
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>643</v>
+      </c>
+      <c r="D4" s="17">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="20">
+        <v>946</v>
+      </c>
+      <c r="D5" s="21">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="20">
+        <v>574</v>
+      </c>
+      <c r="D6" s="21">
+        <v>111</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="20">
+        <v>813</v>
+      </c>
+      <c r="D7" s="21">
+        <v>110</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>793</v>
+      </c>
+      <c r="D8" s="17">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>380</v>
+      </c>
+      <c r="D9" s="17">
+        <v>98</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1">
+        <v>284</v>
+      </c>
+      <c r="D10" s="17">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" s="18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21">
+        <v>92</v>
+      </c>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>106</v>
+      </c>
+      <c r="D12" s="1">
+        <v>91</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="20">
+        <v>127</v>
+      </c>
+      <c r="D13" s="21">
+        <v>90</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A14" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1">
+        <v>208</v>
+      </c>
+      <c r="D14" s="17">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A15" s="8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>105</v>
+      </c>
+      <c r="D15" s="17">
+        <v>90</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A16" s="18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A17" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="17">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A18" s="18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="20">
+        <v>72</v>
+      </c>
+      <c r="D18" s="21">
+        <v>87</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A19" s="8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1">
+        <v>21</v>
+      </c>
+      <c r="D19" s="17">
+        <v>87</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A20" s="18">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A21" s="18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A22" s="8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1">
+        <v>133</v>
+      </c>
+      <c r="D22" s="17">
+        <v>84</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A23" s="18">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A24" s="8">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A25" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-347</v>
+      </c>
+      <c r="D25" s="17">
+        <v>73</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A26" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-556</v>
+      </c>
+      <c r="D26" s="17">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G29" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E26">
+    <sortCondition descending="1" ref="D2:D26"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="G29" r:id="rId1" xr:uid="{A6C2AB78-9D01-493C-9D7D-D0FB49867D7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="8.7265625" style="17"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="88.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1599</v>
+      </c>
+      <c r="D2" s="20">
+        <v>128</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" s="8">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
       <c r="B3" s="17" t="s">
         <v>24</v>
       </c>
@@ -16981,7 +17439,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="8">
-        <f t="shared" ref="A4:A17" si="0">A3+1</f>
+        <f t="shared" ref="A4:A16" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -17016,17 +17474,17 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" s="8">
+      <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="20">
         <v>380</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="21">
         <v>98</v>
       </c>
       <c r="E6" s="17"/>
@@ -17050,17 +17508,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" s="8">
+      <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="20">
         <v>106</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="20">
         <v>91</v>
       </c>
       <c r="E8" s="1"/>
@@ -17071,15 +17529,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>127</v>
+        <v>208</v>
       </c>
       <c r="D9" s="17">
         <v>90</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" s="8">
@@ -17087,17 +17547,15 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1">
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="D10" s="17">
         <v>90</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>49</v>
-      </c>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" s="8">
@@ -17105,15 +17563,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="D11" s="17">
-        <v>90</v>
-      </c>
-      <c r="E11" s="17"/>
+        <v>88</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" s="8">
@@ -17121,14 +17578,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>21</v>
       </c>
       <c r="D12" s="17">
-        <v>88</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>46</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" s="8">
@@ -17136,13 +17594,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="D13" s="17">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E13" s="17"/>
     </row>
@@ -17152,13 +17610,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="D14" s="17">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="17"/>
     </row>
@@ -17168,12 +17623,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-347</v>
       </c>
       <c r="D15" s="17">
-        <v>82</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>73</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" s="8">
@@ -17181,33 +17641,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1">
-        <v>-347</v>
+        <v>-556</v>
       </c>
       <c r="D16" s="17">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A17" s="8">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1">
-        <v>-556</v>
-      </c>
-      <c r="D17" s="17">
-        <v>70</v>
-      </c>
-      <c r="E17" s="17" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPDATE 10.01.22 - Decision Tree Model Completion
</commit_message>
<xml_diff>
--- a/Resources/Super Bowl Analysis.xlsx
+++ b/Resources/Super Bowl Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orich\Desktop\UM Fintech\1_UM_Repositories\Project_2_SuperBowlPrediction\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C088A6-F1A9-4DD6-B653-8085E39AA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15EEF19-0025-44CE-9D4A-5E2F8048B94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7215" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_2011_regular_ season_1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="W" sheetId="3" r:id="rId3"/>
     <sheet name="Selection-W+Net Pts" sheetId="4" r:id="rId4"/>
     <sheet name="Consolidated" sheetId="5" r:id="rId5"/>
-    <sheet name="W3_Sorted-Qualitative Knowl (2)" sheetId="8" r:id="rId6"/>
+    <sheet name="W3_Sorted-Qualitative Knowledge" sheetId="8" r:id="rId6"/>
     <sheet name="W4_Sorted-Qualitative Knowledge" sheetId="6" r:id="rId7"/>
     <sheet name="Final Listing" sheetId="7" r:id="rId8"/>
   </sheets>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="67">
   <si>
     <t>Years</t>
   </si>
@@ -227,12 +227,36 @@
   <si>
     <t>https://www.pro-football-reference.com/years/2022/index.htm</t>
   </si>
+  <si>
+    <t>Wins (+80)</t>
+  </si>
+  <si>
+    <t>Patriots are the only team to win in</t>
+  </si>
+  <si>
+    <t>multiple seasons in last 10 years</t>
+  </si>
+  <si>
+    <t>Repeat Champions</t>
+  </si>
+  <si>
+    <t>One-Time Champions</t>
+  </si>
+  <si>
+    <t>Non- Champions</t>
+  </si>
+  <si>
+    <t>Based on 2022 Week 3</t>
+  </si>
+  <si>
+    <t>Based on 2021 Record</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,6 +410,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -705,6 +735,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -751,7 +898,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -809,10 +956,134 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4763,6 +5034,244 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Arrow: Right 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1ED07DF-A78F-F16E-0686-618B94544BC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5045075" y="1676400"/>
+          <a:ext cx="1676400" cy="739775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>181709</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9794A59B-2DF0-07A7-47F9-9D9228FED809}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5695950"/>
+          <a:ext cx="11765017" cy="5048955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2038350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Arrow: Right 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66CD9066-D943-F677-5C98-558EDAD4BF8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13887451" y="1558925"/>
+          <a:ext cx="1724024" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>327025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>2051049</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Arrow: Right 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E02D308E-0D16-497A-8CC8-C61623AB1335}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20901025" y="1536700"/>
+          <a:ext cx="1724024" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="E7 INVESTMENT GROUP" refreshedDate="44832.92823229167" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="352" xr:uid="{00000000-000A-0000-FFFF-FFFF04000000}">
   <cacheSource type="worksheet">
@@ -9772,7 +10281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D353"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -15559,7 +16068,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -15567,6 +16076,7 @@
     <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.75">
@@ -15574,7 +16084,7 @@
         <v>56</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.75">
@@ -16036,7 +16546,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -16509,7 +17019,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -16527,6 +17037,9 @@
       <c r="D1" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="8">
@@ -16927,7 +17440,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="23" t="s">
         <v>58</v>
       </c>
     </row>
@@ -16944,8 +17457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -16963,6 +17476,9 @@
       <c r="D1" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="8">
@@ -17228,17 +17744,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A18" s="18">
+      <c r="A18" s="24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="26">
         <v>72</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="25">
         <v>87</v>
       </c>
       <c r="E18" s="3"/>
@@ -17363,7 +17879,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="23" t="s">
         <v>58</v>
       </c>
     </row>
@@ -17380,280 +17896,1463 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="B1:AH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="8.7265625" style="17"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" customWidth="1"/>
+    <col min="2" max="2" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="6.7265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="19.40625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.40625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.04296875" customWidth="1"/>
+    <col min="16" max="16" width="12.31640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.40625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.7265625" customWidth="1"/>
+    <col min="22" max="22" width="12.31640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="31.40625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
+    <row r="2" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="61"/>
+    </row>
+    <row r="3" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B3" s="56"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F3" s="51" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="88.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="18">
+      <c r="G3" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3" s="55"/>
+    </row>
+    <row r="4" spans="2:34" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B4" s="56"/>
+      <c r="C4" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20">
+      <c r="E4" s="37">
         <v>1599</v>
       </c>
-      <c r="D2" s="20">
+      <c r="F4" s="37">
         <v>128</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="G4" s="53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" s="8">
-        <f>A2+1</f>
+      <c r="H4" s="57"/>
+      <c r="I4" s="28">
+        <v>1</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="29">
+        <v>1599</v>
+      </c>
+      <c r="L4" s="29">
+        <v>128</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="57"/>
+      <c r="O4" s="28">
+        <v>1</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>1599</v>
+      </c>
+      <c r="R4" s="29">
+        <v>128</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="55"/>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B5" s="56"/>
+      <c r="C5" s="35">
+        <f>C4+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="D5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E5" s="37">
         <v>708</v>
       </c>
-      <c r="D3" s="17">
+      <c r="F5" s="36">
         <v>118</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G5" s="38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" s="8">
-        <f t="shared" ref="A4:A16" si="0">A3+1</f>
+      <c r="H5" s="57"/>
+      <c r="I5" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="55"/>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B6" s="56"/>
+      <c r="C6" s="35">
+        <f t="shared" ref="C6:C19" si="0">C5+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="D6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E6" s="37">
         <v>643</v>
       </c>
-      <c r="D4" s="17">
+      <c r="F6" s="36">
         <v>112</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="G6" s="38" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" s="8">
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="55"/>
+    </row>
+    <row r="7" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B7" s="56"/>
+      <c r="C7" s="35">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="D7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E7" s="37">
         <v>793</v>
       </c>
-      <c r="D5" s="17">
+      <c r="F7" s="36">
         <v>105</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="G7" s="38" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" s="18">
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
+      <c r="Y7" s="57"/>
+      <c r="Z7" s="55"/>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B8" s="56"/>
+      <c r="C8" s="35">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="D8" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="20">
+      <c r="E8" s="37">
         <v>380</v>
       </c>
-      <c r="D6" s="21">
+      <c r="F8" s="36">
         <v>98</v>
       </c>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A7" s="8">
+      <c r="G8" s="38"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="31">
+        <f>I4+1</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="33">
+        <v>708</v>
+      </c>
+      <c r="L8" s="32">
+        <v>118</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="57"/>
+      <c r="O8" s="31">
+        <f>O4+1</f>
+        <v>2</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>708</v>
+      </c>
+      <c r="R8" s="32">
+        <v>118</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="57"/>
+      <c r="U8" s="31">
+        <f>U4+1</f>
+        <v>1</v>
+      </c>
+      <c r="V8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="W8" s="33">
+        <v>708</v>
+      </c>
+      <c r="X8" s="32">
+        <v>118</v>
+      </c>
+      <c r="Y8" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="55"/>
+      <c r="AD8" s="31">
+        <f>AD4+1</f>
+        <v>1</v>
+      </c>
+      <c r="AE8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF8" s="33">
+        <v>708</v>
+      </c>
+      <c r="AG8" s="32">
+        <v>118</v>
+      </c>
+      <c r="AH8" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B9" s="56"/>
+      <c r="C9" s="35">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="D9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E9" s="37">
         <v>284</v>
       </c>
-      <c r="D7" s="17">
+      <c r="F9" s="36">
         <v>97</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="G9" s="38" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" s="18">
+      <c r="H9" s="57"/>
+      <c r="I9" s="35">
+        <f t="shared" ref="I9:I24" si="1">I8+1</f>
+        <v>3</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="37">
+        <v>643</v>
+      </c>
+      <c r="L9" s="36">
+        <v>112</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="57"/>
+      <c r="O9" s="35">
+        <f t="shared" ref="O9" si="2">O8+1</f>
+        <v>3</v>
+      </c>
+      <c r="P9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="37">
+        <v>643</v>
+      </c>
+      <c r="R9" s="36">
+        <v>112</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" s="57"/>
+      <c r="U9" s="35">
+        <f t="shared" ref="U9" si="3">U8+1</f>
+        <v>2</v>
+      </c>
+      <c r="V9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="37">
+        <v>643</v>
+      </c>
+      <c r="X9" s="36">
+        <v>112</v>
+      </c>
+      <c r="Y9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z9" s="55"/>
+      <c r="AD9" s="35">
+        <f t="shared" ref="AD9" si="4">AD8+1</f>
+        <v>2</v>
+      </c>
+      <c r="AE9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="37">
+        <v>643</v>
+      </c>
+      <c r="AG9" s="36">
+        <v>112</v>
+      </c>
+      <c r="AH9" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B10" s="56"/>
+      <c r="C10" s="35">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="D10" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="20">
+      <c r="E10" s="37">
         <v>106</v>
       </c>
-      <c r="D8" s="20">
+      <c r="F10" s="37">
         <v>91</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A9" s="8">
+      <c r="G10" s="46"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="37">
+        <v>793</v>
+      </c>
+      <c r="L10" s="36">
+        <v>105</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="57"/>
+      <c r="O10" s="35">
+        <f>O9+1</f>
+        <v>4</v>
+      </c>
+      <c r="P10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="37">
+        <v>284</v>
+      </c>
+      <c r="R10" s="36">
+        <v>97</v>
+      </c>
+      <c r="S10" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="T10" s="57"/>
+      <c r="U10" s="35">
+        <f>U9+1</f>
+        <v>3</v>
+      </c>
+      <c r="V10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" s="37">
+        <v>284</v>
+      </c>
+      <c r="X10" s="36">
+        <v>97</v>
+      </c>
+      <c r="Y10" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z10" s="55"/>
+      <c r="AD10" s="35">
+        <f>AD9+1</f>
+        <v>3</v>
+      </c>
+      <c r="AE10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF10" s="37">
+        <v>284</v>
+      </c>
+      <c r="AG10" s="36">
+        <v>97</v>
+      </c>
+      <c r="AH10" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B11" s="56"/>
+      <c r="C11" s="54">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="D11" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E11" s="40">
         <v>208</v>
       </c>
-      <c r="D9" s="17">
+      <c r="F11" s="39">
         <v>90</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="G11" s="41" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A10" s="8">
+      <c r="H11" s="40"/>
+      <c r="I11" s="35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="37">
+        <v>284</v>
+      </c>
+      <c r="L11" s="36">
+        <v>97</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="57"/>
+      <c r="O11" s="35">
+        <f>O10+1</f>
+        <v>5</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="40">
+        <v>208</v>
+      </c>
+      <c r="R11" s="39">
+        <v>90</v>
+      </c>
+      <c r="S11" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" s="57"/>
+      <c r="U11" s="35">
+        <f>U10+1</f>
+        <v>4</v>
+      </c>
+      <c r="V11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="W11" s="40">
+        <v>208</v>
+      </c>
+      <c r="X11" s="39">
+        <v>90</v>
+      </c>
+      <c r="Y11" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="55"/>
+      <c r="AD11" s="35">
+        <f>AD10+1</f>
+        <v>4</v>
+      </c>
+      <c r="AE11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF11" s="40">
+        <v>208</v>
+      </c>
+      <c r="AG11" s="39">
+        <v>90</v>
+      </c>
+      <c r="AH11" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B12" s="56"/>
+      <c r="C12" s="54">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="D12" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E12" s="40">
         <v>105</v>
       </c>
-      <c r="D10" s="17">
+      <c r="F12" s="39">
         <v>90</v>
       </c>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A11" s="8">
+      <c r="G12" s="41"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="40">
+        <v>208</v>
+      </c>
+      <c r="L12" s="39">
+        <v>90</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="57"/>
+      <c r="O12" s="35">
+        <f t="shared" ref="O12:O13" si="5">O11+1</f>
+        <v>6</v>
+      </c>
+      <c r="P12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="40">
+        <v>-43</v>
+      </c>
+      <c r="R12" s="39">
+        <v>88</v>
+      </c>
+      <c r="S12" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12" s="57"/>
+      <c r="U12" s="35">
+        <f t="shared" ref="U12:U13" si="6">U11+1</f>
+        <v>5</v>
+      </c>
+      <c r="V12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="W12" s="40">
+        <v>-43</v>
+      </c>
+      <c r="X12" s="39">
+        <v>88</v>
+      </c>
+      <c r="Y12" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z12" s="55"/>
+      <c r="AD12" s="35">
+        <f t="shared" ref="AD12:AD17" si="7">AD11+1</f>
+        <v>5</v>
+      </c>
+      <c r="AE12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF12" s="40">
+        <v>-43</v>
+      </c>
+      <c r="AG12" s="39">
+        <v>88</v>
+      </c>
+      <c r="AH12" s="41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B13" s="56"/>
+      <c r="C13" s="54">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="D13" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="17">
+      <c r="E13" s="40">
+        <v>-43</v>
+      </c>
+      <c r="F13" s="39">
         <v>88</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="G13" s="41" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A12" s="8">
+      <c r="H13" s="57"/>
+      <c r="I13" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="40">
+        <v>-43</v>
+      </c>
+      <c r="L13" s="39">
+        <v>88</v>
+      </c>
+      <c r="M13" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="57"/>
+      <c r="O13" s="42">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="44">
+        <v>-347</v>
+      </c>
+      <c r="R13" s="43">
+        <v>73</v>
+      </c>
+      <c r="S13" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="T13" s="57"/>
+      <c r="U13" s="42">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="V13" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="W13" s="44">
+        <v>-347</v>
+      </c>
+      <c r="X13" s="43">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13" s="55"/>
+      <c r="AD13" s="35">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="AE13" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF13" s="40">
+        <v>-347</v>
+      </c>
+      <c r="AG13" s="39">
+        <v>73</v>
+      </c>
+      <c r="AH13" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B14" s="56"/>
+      <c r="C14" s="54">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="D14" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E14" s="40">
         <v>21</v>
       </c>
-      <c r="D12" s="17">
+      <c r="F14" s="39">
         <v>87</v>
       </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A13" s="8">
+      <c r="G14" s="41"/>
+      <c r="H14" s="72" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="40">
+        <v>-347</v>
+      </c>
+      <c r="L14" s="39">
+        <v>73</v>
+      </c>
+      <c r="M14" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="57"/>
+      <c r="Z14" s="55"/>
+      <c r="AD14" s="35">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="AE14" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF14" s="37">
+        <v>380</v>
+      </c>
+      <c r="AG14" s="36">
+        <v>98</v>
+      </c>
+      <c r="AH14" s="55"/>
+    </row>
+    <row r="15" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B15" s="56"/>
+      <c r="C15" s="54">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
-        <v>133</v>
-      </c>
-      <c r="D13" s="17">
-        <v>84</v>
-      </c>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A14" s="8">
+      <c r="D15" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="37">
+        <v>72</v>
+      </c>
+      <c r="F15" s="36">
+        <v>87</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="42">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="44">
+        <v>-556</v>
+      </c>
+      <c r="L15" s="43">
+        <v>70</v>
+      </c>
+      <c r="M15" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
+      <c r="Y15" s="57"/>
+      <c r="Z15" s="55"/>
+      <c r="AD15" s="35">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AE15" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF15" s="37">
+        <v>106</v>
+      </c>
+      <c r="AG15" s="37">
+        <v>91</v>
+      </c>
+      <c r="AH15" s="55"/>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B16" s="56"/>
+      <c r="C16" s="54">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="17">
-        <v>82</v>
-      </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A15" s="8">
+      <c r="D16" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="40">
+        <v>133</v>
+      </c>
+      <c r="F16" s="39">
+        <v>84</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="55"/>
+      <c r="AD16" s="35">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AE16" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF16" s="40">
+        <v>105</v>
+      </c>
+      <c r="AG16" s="39">
+        <v>90</v>
+      </c>
+      <c r="AH16" s="55"/>
+    </row>
+    <row r="17" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B17" s="56"/>
+      <c r="C17" s="54">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-347</v>
-      </c>
-      <c r="D15" s="17">
-        <v>73</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A16" s="8">
+      <c r="D17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="40">
+        <v>-492</v>
+      </c>
+      <c r="F17" s="39">
+        <v>82</v>
+      </c>
+      <c r="G17" s="55"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="57"/>
+      <c r="Z17" s="55"/>
+      <c r="AD17" s="42">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AE17" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF17" s="63">
+        <v>72</v>
+      </c>
+      <c r="AG17" s="65">
+        <v>87</v>
+      </c>
+      <c r="AH17" s="47"/>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B18" s="56"/>
+      <c r="C18" s="54">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="D18" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="40">
+        <v>-347</v>
+      </c>
+      <c r="F18" s="39">
+        <v>73</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="57"/>
+      <c r="I18" s="31">
+        <v>10</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="33">
+        <v>380</v>
+      </c>
+      <c r="L18" s="32">
+        <v>98</v>
+      </c>
+      <c r="M18" s="34"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="31">
+        <f>O13+1</f>
+        <v>8</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="33">
+        <v>380</v>
+      </c>
+      <c r="R18" s="32">
+        <v>98</v>
+      </c>
+      <c r="S18" s="61"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="31">
+        <f>U13+1</f>
+        <v>7</v>
+      </c>
+      <c r="V18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="W18" s="33">
+        <v>380</v>
+      </c>
+      <c r="X18" s="34">
+        <v>98</v>
+      </c>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="55"/>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B19" s="56"/>
+      <c r="C19" s="54">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1">
+      <c r="E19" s="40">
         <v>-556</v>
       </c>
-      <c r="D16" s="17">
+      <c r="F19" s="39">
         <v>70</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="G19" s="41" t="s">
         <v>54</v>
       </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="35">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="37">
+        <v>106</v>
+      </c>
+      <c r="L19" s="37">
+        <v>91</v>
+      </c>
+      <c r="M19" s="46"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="35">
+        <f t="shared" ref="O19" si="8">O18+1</f>
+        <v>9</v>
+      </c>
+      <c r="P19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="37">
+        <v>106</v>
+      </c>
+      <c r="R19" s="37">
+        <v>91</v>
+      </c>
+      <c r="S19" s="55"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="35">
+        <f t="shared" ref="U19:U21" si="9">U18+1</f>
+        <v>8</v>
+      </c>
+      <c r="V19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" s="37">
+        <v>106</v>
+      </c>
+      <c r="X19" s="46">
+        <v>91</v>
+      </c>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="55"/>
+    </row>
+    <row r="20" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="35">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="40">
+        <v>105</v>
+      </c>
+      <c r="L20" s="39">
+        <v>90</v>
+      </c>
+      <c r="M20" s="41"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="35">
+        <f t="shared" ref="O20:O23" si="10">O19+1</f>
+        <v>10</v>
+      </c>
+      <c r="P20" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="40">
+        <v>105</v>
+      </c>
+      <c r="R20" s="39">
+        <v>90</v>
+      </c>
+      <c r="S20" s="55"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="35">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="V20" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="W20" s="40">
+        <v>105</v>
+      </c>
+      <c r="X20" s="41">
+        <v>90</v>
+      </c>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="55"/>
+    </row>
+    <row r="21" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="35">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="40">
+        <v>21</v>
+      </c>
+      <c r="L21" s="39">
+        <v>87</v>
+      </c>
+      <c r="M21" s="41"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="35">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="37">
+        <v>72</v>
+      </c>
+      <c r="R21" s="36">
+        <v>87</v>
+      </c>
+      <c r="S21" s="55"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="42">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="V21" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="W21" s="63">
+        <v>72</v>
+      </c>
+      <c r="X21" s="64">
+        <v>87</v>
+      </c>
+      <c r="Y21" s="57"/>
+      <c r="Z21" s="55"/>
+    </row>
+    <row r="22" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="35">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J22" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="37">
+        <v>72</v>
+      </c>
+      <c r="L22" s="36">
+        <v>87</v>
+      </c>
+      <c r="M22" s="41"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="35">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="P22" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="62">
+        <v>-284</v>
+      </c>
+      <c r="R22" s="62">
+        <v>86</v>
+      </c>
+      <c r="S22" s="55"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="55"/>
+    </row>
+    <row r="23" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B23" s="56"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="35">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="40">
+        <v>133</v>
+      </c>
+      <c r="L23" s="39">
+        <v>84</v>
+      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="42">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="P23" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="44">
+        <v>-492</v>
+      </c>
+      <c r="R23" s="43">
+        <v>82</v>
+      </c>
+      <c r="S23" s="47"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="55"/>
+    </row>
+    <row r="24" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B24" s="56"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="42">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" s="44">
+        <v>-492</v>
+      </c>
+      <c r="L24" s="43">
+        <v>82</v>
+      </c>
+      <c r="M24" s="47"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="55"/>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.75">
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="55"/>
+    </row>
+    <row r="26" spans="2:34" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B26" s="59"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="60"/>
+      <c r="S26" s="60"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="60"/>
+      <c r="V26" s="60"/>
+      <c r="W26" s="60"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="47"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I4:L13">
+    <sortCondition descending="1" ref="K4:K13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>